<commit_message>
everyone filled in the survey
</commit_message>
<xml_diff>
--- a/data analysis (version 1).xlsx
+++ b/data analysis (version 1).xlsx
@@ -736,10 +736,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Survey Data'!$D$32:$D$38</c:f>
+              <c:f>'Survey Data'!$D$32:$D$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>8.0</c:v>
                 </c:pt>
@@ -759,6 +759,9 @@
                   <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>9.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -782,10 +785,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Survey Data'!$E$32:$E$38</c:f>
+              <c:f>'Survey Data'!$E$32:$E$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>8.0</c:v>
                 </c:pt>
@@ -806,6 +809,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -828,10 +834,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Survey Data'!$F$32:$F$38</c:f>
+              <c:f>'Survey Data'!$F$32:$F$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>9.0</c:v>
                 </c:pt>
@@ -852,6 +858,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -874,10 +883,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Survey Data'!$G$32:$G$38</c:f>
+              <c:f>'Survey Data'!$G$32:$G$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>8.0</c:v>
                 </c:pt>
@@ -898,6 +907,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -920,10 +932,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Survey Data'!$H$32:$H$38</c:f>
+              <c:f>'Survey Data'!$H$32:$H$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>8.0</c:v>
                 </c:pt>
@@ -944,6 +956,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1748,10 +1763,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M38"/>
+  <dimension ref="B2:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView tabSelected="1" topLeftCell="J19" workbookViewId="0">
+      <selection activeCell="M57" sqref="M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1857,10 +1872,14 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="2:13" ht="16">
-      <c r="B10" s="3"/>
+      <c r="B10" s="3">
+        <v>9</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3">
+        <v>8</v>
+      </c>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="2:13" ht="16">
@@ -1967,7 +1986,9 @@
       </c>
     </row>
     <row r="19" spans="2:13" ht="16">
-      <c r="B19" s="3"/>
+      <c r="B19" s="3">
+        <v>8</v>
+      </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -2087,6 +2108,14 @@
       </c>
       <c r="F27" s="3"/>
     </row>
+    <row r="28" spans="2:13" ht="16">
+      <c r="B28" s="3">
+        <v>7</v>
+      </c>
+      <c r="E28" s="3">
+        <v>5</v>
+      </c>
+    </row>
     <row r="31" spans="2:13">
       <c r="D31" t="s">
         <v>24</v>
@@ -2221,6 +2250,23 @@
       </c>
       <c r="H38" s="3">
         <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="4:8" ht="16">
+      <c r="D39" s="3">
+        <v>9</v>
+      </c>
+      <c r="E39" s="3">
+        <v>8</v>
+      </c>
+      <c r="F39" s="3">
+        <v>8</v>
+      </c>
+      <c r="G39" s="3">
+        <v>7</v>
+      </c>
+      <c r="H39" s="3">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>